<commit_message>
fluff plus minor stuff :)
</commit_message>
<xml_diff>
--- a/optim-stratif/Testing_outputs/tests.xlsx
+++ b/optim-stratif/Testing_outputs/tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>nh</t>
   </si>
@@ -81,7 +81,13 @@
     <t>Design_var</t>
   </si>
   <si>
-    <t>St.Dev.</t>
+    <t xml:space="preserve">Therefore RMSE^2 in output is the design variance :) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">St.Dev. (or RMSE :)) </t>
+  </si>
+  <si>
+    <t>desvar</t>
   </si>
 </sst>
 </file>
@@ -690,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R1447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -850,6 +856,9 @@
         <f>VAR(E2:E1447)</f>
         <v>0.81816028176458144</v>
       </c>
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4">
@@ -960,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1153,6 +1162,12 @@
       <c r="J10">
         <v>5</v>
       </c>
+      <c r="L10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11">
@@ -1184,6 +1199,12 @@
       </c>
       <c r="J11">
         <v>5</v>
+      </c>
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11">
+        <v>2.86E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18">

</xml_diff>